<commit_message>
Adding high level interactions diagram and updating listeners flows
</commit_message>
<xml_diff>
--- a/docs/flow/broadcast_partner_information.xlsx
+++ b/docs/flow/broadcast_partner_information.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthurthev/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunoric/Devel/Smartbox/millenniumfalcon/r2-d2-api/docs/flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F909B36-7C77-4CF2-950A-DBB057CDC96F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65236F59-E82C-4A4C-BBDB-85B04FAE09CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="352">
   <si>
     <t>Integration Information</t>
   </si>
@@ -1078,13 +1078,25 @@
   </si>
   <si>
     <t>API Response Field</t>
+  </si>
+  <si>
+    <t>R2D2 Partner Calendar</t>
+  </si>
+  <si>
+    <t>/broadcast_listerners/partners</t>
+  </si>
+  <si>
+    <t>smartbox_id</t>
+  </si>
+  <si>
+    <t>partners</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1609,7 +1621,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1701,9 +1713,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="3" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="3" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1714,30 +1723,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1833,6 +1818,30 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -2122,93 +2131,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="Q19" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.125" style="2" customWidth="1"/>
-    <col min="2" max="9" width="23.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" style="2" customWidth="1"/>
+    <col min="2" max="9" width="23.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="33.5" style="2" customWidth="1"/>
-    <col min="11" max="15" width="23.625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="27.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="22" width="23.625" style="2" customWidth="1"/>
+    <col min="11" max="15" width="23.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="23.6640625" style="2" customWidth="1"/>
     <col min="23" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="48"/>
-    </row>
-    <row r="2" spans="1:22">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="51"/>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
-    </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1">
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="60"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="53"/>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2227,18 +2236,18 @@
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="56"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -2254,68 +2263,68 @@
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="66"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
       <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
-    </row>
-    <row r="10" spans="1:22">
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
       <c r="H10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
       <c r="H11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -2343,107 +2352,111 @@
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="45"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="45"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="44" t="s">
+      <c r="I14" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="45"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="44" t="s">
+      <c r="L14" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="45"/>
+      <c r="M14" s="38"/>
       <c r="N14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="44" t="s">
+      <c r="O14" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="P14" s="45"/>
+      <c r="P14" s="38"/>
       <c r="Q14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="R14" s="44" t="s">
+      <c r="R14" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="S14" s="45"/>
+      <c r="S14" s="38"/>
       <c r="T14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="U14" s="44"/>
-      <c r="V14" s="45"/>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="U14" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="V14" s="38"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="37" t="s">
+      <c r="D15" s="38"/>
+      <c r="E15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="37" t="s">
+      <c r="G15" s="38"/>
+      <c r="H15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="44"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="37" t="s">
+      <c r="I15" s="37"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="44"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="37" t="s">
+      <c r="L15" s="37"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="O15" s="44" t="s">
+      <c r="O15" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="37" t="s">
+      <c r="P15" s="38"/>
+      <c r="Q15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="R15" s="44" t="s">
+      <c r="R15" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="S15" s="45"/>
-      <c r="T15" s="37" t="s">
+      <c r="S15" s="38"/>
+      <c r="T15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="U15" s="44"/>
-      <c r="V15" s="45"/>
-    </row>
-    <row r="16" spans="1:22">
+      <c r="U15" s="37" t="s">
+        <v>349</v>
+      </c>
+      <c r="V15" s="38"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -2511,7 +2524,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>42</v>
       </c>
@@ -2561,11 +2574,17 @@
         <v>42</v>
       </c>
       <c r="S17" s="20"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="T17" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="U17" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="V17" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>52</v>
       </c>
@@ -2615,11 +2634,17 @@
         <v>52</v>
       </c>
       <c r="S18" s="20"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="T18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V18" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>59</v>
       </c>
@@ -2669,11 +2694,17 @@
         <v>59</v>
       </c>
       <c r="S19" s="20"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="T19" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U19" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V19" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>64</v>
       </c>
@@ -2721,11 +2752,17 @@
         <v>64</v>
       </c>
       <c r="S20" s="20"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="19"/>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="T20" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="U20" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="V20" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>71</v>
       </c>
@@ -2771,11 +2808,17 @@
         <v>71</v>
       </c>
       <c r="S21" s="20"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="T21" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U21" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V21" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>73</v>
       </c>
@@ -2825,11 +2868,17 @@
         <v>73</v>
       </c>
       <c r="S22" s="20"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="T22" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U22" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V22" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>80</v>
       </c>
@@ -2879,11 +2928,17 @@
         <v>80</v>
       </c>
       <c r="S23" s="20"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="T23" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U23" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V23" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>85</v>
       </c>
@@ -2933,11 +2988,17 @@
         <v>85</v>
       </c>
       <c r="S24" s="20"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="T24" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="U24" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="V24" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>92</v>
       </c>
@@ -2987,11 +3048,17 @@
         <v>97</v>
       </c>
       <c r="S25" s="20"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="T25" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U25" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V25" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>98</v>
       </c>
@@ -3041,11 +3108,17 @@
         <v>103</v>
       </c>
       <c r="S26" s="20"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-    </row>
-    <row r="27" spans="1:22">
+      <c r="T26" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U26" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V26" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>104</v>
       </c>
@@ -3095,11 +3168,17 @@
         <v>104</v>
       </c>
       <c r="S27" s="20"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19"/>
-    </row>
-    <row r="28" spans="1:22">
+      <c r="T27" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U27" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V27" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>109</v>
       </c>
@@ -3149,11 +3228,17 @@
         <v>109</v>
       </c>
       <c r="S28" s="20"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-    </row>
-    <row r="29" spans="1:22">
+      <c r="T28" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U28" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V28" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>115</v>
       </c>
@@ -3203,11 +3288,17 @@
         <v>115</v>
       </c>
       <c r="S29" s="20"/>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
-    </row>
-    <row r="30" spans="1:22">
+      <c r="T29" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U29" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V29" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>122</v>
       </c>
@@ -3257,11 +3348,17 @@
         <v>128</v>
       </c>
       <c r="S30" s="20"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-    </row>
-    <row r="31" spans="1:22">
+      <c r="T30" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U30" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V30" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>129</v>
       </c>
@@ -3311,11 +3408,17 @@
         <v>133</v>
       </c>
       <c r="S31" s="20"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-    </row>
-    <row r="32" spans="1:22">
+      <c r="T31" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U31" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V31" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>134</v>
       </c>
@@ -3365,11 +3468,17 @@
         <v>138</v>
       </c>
       <c r="S32" s="20"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-    </row>
-    <row r="33" spans="1:22">
+      <c r="T32" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U32" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V32" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>139</v>
       </c>
@@ -3419,11 +3528,17 @@
         <v>144</v>
       </c>
       <c r="S33" s="20"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-    </row>
-    <row r="34" spans="1:22">
+      <c r="T33" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U33" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V33" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>145</v>
       </c>
@@ -3473,11 +3588,17 @@
         <v>150</v>
       </c>
       <c r="S34" s="20"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-    </row>
-    <row r="35" spans="1:22">
+      <c r="T34" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U34" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V34" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>151</v>
       </c>
@@ -3527,11 +3648,17 @@
         <v>156</v>
       </c>
       <c r="S35" s="20"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-    </row>
-    <row r="36" spans="1:22">
+      <c r="T35" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U35" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V35" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>157</v>
       </c>
@@ -3581,11 +3708,17 @@
         <v>162</v>
       </c>
       <c r="S36" s="20"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="19"/>
-    </row>
-    <row r="37" spans="1:22">
+      <c r="T36" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U36" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V36" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>163</v>
       </c>
@@ -3635,11 +3768,17 @@
         <v>168</v>
       </c>
       <c r="S37" s="20"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-    </row>
-    <row r="38" spans="1:22">
+      <c r="T37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V37" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>169</v>
       </c>
@@ -3689,11 +3828,17 @@
         <v>174</v>
       </c>
       <c r="S38" s="20"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-    </row>
-    <row r="39" spans="1:22">
+      <c r="T38" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U38" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V38" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>175</v>
       </c>
@@ -3743,11 +3888,17 @@
         <v>180</v>
       </c>
       <c r="S39" s="20"/>
-      <c r="T39" s="19"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="19"/>
-    </row>
-    <row r="40" spans="1:22">
+      <c r="T39" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U39" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V39" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>181</v>
       </c>
@@ -3797,11 +3948,17 @@
         <v>186</v>
       </c>
       <c r="S40" s="20"/>
-      <c r="T40" s="19"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="19"/>
-    </row>
-    <row r="41" spans="1:22">
+      <c r="T40" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U40" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V40" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>187</v>
       </c>
@@ -3850,11 +4007,17 @@
         <v>193</v>
       </c>
       <c r="S41" s="20"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-    </row>
-    <row r="42" spans="1:22">
+      <c r="T41" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U41" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V41" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
         <v>194</v>
       </c>
@@ -3905,11 +4068,17 @@
         <v>200</v>
       </c>
       <c r="S42" s="20"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-    </row>
-    <row r="43" spans="1:22">
+      <c r="T42" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U42" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V42" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>201</v>
       </c>
@@ -3960,11 +4129,17 @@
         <v>206</v>
       </c>
       <c r="S43" s="20"/>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-    </row>
-    <row r="44" spans="1:22">
+      <c r="T43" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U43" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V43" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
         <v>207</v>
       </c>
@@ -4015,11 +4190,17 @@
         <v>213</v>
       </c>
       <c r="S44" s="20"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-    </row>
-    <row r="45" spans="1:22">
+      <c r="T44" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U44" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V44" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>214</v>
       </c>
@@ -4068,11 +4249,17 @@
         <v>219</v>
       </c>
       <c r="S45" s="20"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-    </row>
-    <row r="46" spans="1:22">
+      <c r="T45" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U45" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V45" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
         <v>220</v>
       </c>
@@ -4119,11 +4306,17 @@
         <v>223</v>
       </c>
       <c r="S46" s="20"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-    </row>
-    <row r="47" spans="1:22">
+      <c r="T46" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U46" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V46" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>224</v>
       </c>
@@ -4170,11 +4363,17 @@
         <v>228</v>
       </c>
       <c r="S47" s="20"/>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-    </row>
-    <row r="48" spans="1:22">
+      <c r="T47" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U47" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V47" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>229</v>
       </c>
@@ -4210,11 +4409,17 @@
       <c r="Q48" s="20"/>
       <c r="R48" s="20"/>
       <c r="S48" s="20"/>
-      <c r="T48" s="19"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="19"/>
-    </row>
-    <row r="49" spans="1:22">
+      <c r="T48" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U48" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V48" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
         <v>235</v>
       </c>
@@ -4250,11 +4455,17 @@
         <v>238</v>
       </c>
       <c r="S49" s="20"/>
-      <c r="T49" s="19"/>
-      <c r="U49" s="19"/>
-      <c r="V49" s="19"/>
-    </row>
-    <row r="50" spans="1:22">
+      <c r="T49" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U49" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V49" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
         <v>239</v>
       </c>
@@ -4305,11 +4516,17 @@
         <v>244</v>
       </c>
       <c r="S50" s="20"/>
-      <c r="T50" s="19"/>
-      <c r="U50" s="19"/>
-      <c r="V50" s="19"/>
-    </row>
-    <row r="51" spans="1:22">
+      <c r="T50" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U50" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V50" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
         <v>245</v>
       </c>
@@ -4360,11 +4577,17 @@
         <v>251</v>
       </c>
       <c r="S51" s="20"/>
-      <c r="T51" s="19"/>
-      <c r="U51" s="19"/>
-      <c r="V51" s="19"/>
-    </row>
-    <row r="52" spans="1:22">
+      <c r="T51" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U51" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V51" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
         <v>252</v>
       </c>
@@ -4415,11 +4638,17 @@
         <v>257</v>
       </c>
       <c r="S52" s="20"/>
-      <c r="T52" s="19"/>
-      <c r="U52" s="19"/>
-      <c r="V52" s="19"/>
-    </row>
-    <row r="53" spans="1:22">
+      <c r="T52" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U52" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V52" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
         <v>258</v>
       </c>
@@ -4469,11 +4698,17 @@
         <v>264</v>
       </c>
       <c r="S53" s="20"/>
-      <c r="T53" s="19"/>
-      <c r="U53" s="19"/>
-      <c r="V53" s="19"/>
-    </row>
-    <row r="54" spans="1:22">
+      <c r="T53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V53" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
         <v>265</v>
       </c>
@@ -4523,11 +4758,17 @@
         <v>270</v>
       </c>
       <c r="S54" s="20"/>
-      <c r="T54" s="19"/>
-      <c r="U54" s="19"/>
-      <c r="V54" s="19"/>
-    </row>
-    <row r="55" spans="1:22">
+      <c r="T54" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U54" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V54" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
         <v>271</v>
       </c>
@@ -4578,11 +4819,17 @@
         <v>278</v>
       </c>
       <c r="S55" s="20"/>
-      <c r="T55" s="19"/>
-      <c r="U55" s="19"/>
-      <c r="V55" s="19"/>
-    </row>
-    <row r="56" spans="1:22">
+      <c r="T55" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U55" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V55" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
         <v>279</v>
       </c>
@@ -4630,11 +4877,17 @@
         <v>279</v>
       </c>
       <c r="S56" s="20"/>
-      <c r="T56" s="19"/>
-      <c r="U56" s="19"/>
-      <c r="V56" s="19"/>
-    </row>
-    <row r="57" spans="1:22">
+      <c r="T56" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U56" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V56" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
         <v>284</v>
       </c>
@@ -4684,11 +4937,17 @@
         <v>284</v>
       </c>
       <c r="S57" s="20"/>
-      <c r="T57" s="19"/>
-      <c r="U57" s="19"/>
-      <c r="V57" s="19"/>
-    </row>
-    <row r="58" spans="1:22">
+      <c r="T57" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U57" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V57" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
         <v>290</v>
       </c>
@@ -4735,11 +4994,17 @@
         <v>293</v>
       </c>
       <c r="S58" s="20"/>
-      <c r="T58" s="19"/>
-      <c r="U58" s="19"/>
-      <c r="V58" s="19"/>
-    </row>
-    <row r="59" spans="1:22">
+      <c r="T58" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U58" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V58" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
         <v>294</v>
       </c>
@@ -4786,11 +5051,17 @@
         <v>298</v>
       </c>
       <c r="S59" s="20"/>
-      <c r="T59" s="19"/>
-      <c r="U59" s="19"/>
-      <c r="V59" s="19"/>
-    </row>
-    <row r="60" spans="1:22">
+      <c r="T59" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U59" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V59" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
         <v>299</v>
       </c>
@@ -4837,11 +5108,17 @@
         <v>303</v>
       </c>
       <c r="S60" s="20"/>
-      <c r="T60" s="19"/>
-      <c r="U60" s="19"/>
-      <c r="V60" s="19"/>
-    </row>
-    <row r="61" spans="1:22">
+      <c r="T60" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U60" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V60" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
         <v>304</v>
       </c>
@@ -4886,11 +5163,17 @@
         <v>308</v>
       </c>
       <c r="S61" s="20"/>
-      <c r="T61" s="19"/>
-      <c r="U61" s="19"/>
-      <c r="V61" s="19"/>
-    </row>
-    <row r="62" spans="1:22">
+      <c r="T61" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U61" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V61" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
         <v>309</v>
       </c>
@@ -4935,11 +5218,17 @@
         <v>313</v>
       </c>
       <c r="S62" s="20"/>
-      <c r="T62" s="19"/>
-      <c r="U62" s="19"/>
-      <c r="V62" s="19"/>
-    </row>
-    <row r="63" spans="1:22">
+      <c r="T62" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U62" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V62" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
         <v>314</v>
       </c>
@@ -4986,11 +5275,17 @@
         <v>314</v>
       </c>
       <c r="S63" s="20"/>
-      <c r="T63" s="19"/>
-      <c r="U63" s="19"/>
-      <c r="V63" s="19"/>
-    </row>
-    <row r="64" spans="1:22">
+      <c r="T63" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U63" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V63" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
         <v>317</v>
       </c>
@@ -5034,11 +5329,17 @@
         <v>317</v>
       </c>
       <c r="S64" s="20"/>
-      <c r="T64" s="19"/>
-      <c r="U64" s="19"/>
-      <c r="V64" s="19"/>
-    </row>
-    <row r="65" spans="1:22">
+      <c r="T64" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U64" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V64" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
         <v>321</v>
       </c>
@@ -5082,11 +5383,17 @@
         <v>321</v>
       </c>
       <c r="S65" s="20"/>
-      <c r="T65" s="19"/>
-      <c r="U65" s="19"/>
-      <c r="V65" s="19"/>
-    </row>
-    <row r="66" spans="1:22">
+      <c r="T65" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U65" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V65" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
         <v>326</v>
       </c>
@@ -5130,11 +5437,17 @@
         <v>326</v>
       </c>
       <c r="S66" s="29"/>
-      <c r="T66" s="19"/>
-      <c r="U66" s="19"/>
-      <c r="V66" s="19"/>
-    </row>
-    <row r="67" spans="1:22">
+      <c r="T66" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U66" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V66" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
         <v>209</v>
       </c>
@@ -5171,18 +5484,24 @@
       <c r="N67" s="19"/>
       <c r="O67" s="19"/>
       <c r="P67" s="30"/>
-      <c r="Q67" s="35" t="s">
+      <c r="Q67" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="R67" s="35" t="s">
+      <c r="R67" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="S67" s="35"/>
-      <c r="T67" s="32"/>
-      <c r="U67" s="19"/>
-      <c r="V67" s="19"/>
-    </row>
-    <row r="68" spans="1:22">
+      <c r="S67" s="34"/>
+      <c r="T67" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U67" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V67" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
         <v>332</v>
       </c>
@@ -5207,18 +5526,24 @@
       <c r="N68" s="19"/>
       <c r="O68" s="19"/>
       <c r="P68" s="30"/>
-      <c r="Q68" s="35" t="s">
+      <c r="Q68" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="R68" s="35" t="s">
+      <c r="R68" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="S68" s="35"/>
-      <c r="T68" s="32"/>
-      <c r="U68" s="19"/>
-      <c r="V68" s="19"/>
-    </row>
-    <row r="69" spans="1:22" ht="15.75">
+      <c r="S68" s="34"/>
+      <c r="T68" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U68" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V68" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
         <v>335</v>
       </c>
@@ -5243,18 +5568,24 @@
       <c r="N69" s="19"/>
       <c r="O69" s="19"/>
       <c r="P69" s="30"/>
-      <c r="Q69" s="35" t="s">
+      <c r="Q69" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="R69" s="35" t="s">
+      <c r="R69" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="S69" s="35"/>
-      <c r="T69" s="32"/>
-      <c r="U69" s="19"/>
-      <c r="V69" s="19"/>
-    </row>
-    <row r="70" spans="1:22">
+      <c r="S69" s="34"/>
+      <c r="T69" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U69" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V69" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
         <v>338</v>
       </c>
@@ -5279,16 +5610,22 @@
       <c r="N70" s="28"/>
       <c r="O70" s="28"/>
       <c r="P70" s="31"/>
-      <c r="Q70" s="35"/>
-      <c r="R70" s="35" t="s">
+      <c r="Q70" s="34"/>
+      <c r="R70" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="S70" s="35"/>
-      <c r="T70" s="33"/>
-      <c r="U70" s="28"/>
-      <c r="V70" s="28"/>
-    </row>
-    <row r="71" spans="1:22">
+      <c r="S70" s="34"/>
+      <c r="T70" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U70" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V70" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
         <v>341</v>
       </c>
@@ -5307,18 +5644,24 @@
       <c r="N71" s="28"/>
       <c r="O71" s="28"/>
       <c r="P71" s="31"/>
-      <c r="Q71" s="35" t="s">
+      <c r="Q71" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="R71" s="35" t="s">
+      <c r="R71" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="S71" s="35"/>
-      <c r="T71" s="33"/>
-      <c r="U71" s="28"/>
-      <c r="V71" s="28"/>
-    </row>
-    <row r="72" spans="1:22" ht="15.75">
+      <c r="S71" s="34"/>
+      <c r="T71" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="U71" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="V71" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
         <v>342</v>
       </c>
@@ -5349,14 +5692,14 @@
       <c r="N72" s="28"/>
       <c r="O72" s="28"/>
       <c r="P72" s="31"/>
-      <c r="Q72" s="36"/>
-      <c r="R72" s="36"/>
-      <c r="S72" s="36"/>
-      <c r="T72" s="33"/>
+      <c r="Q72" s="35"/>
+      <c r="R72" s="35"/>
+      <c r="S72" s="35"/>
+      <c r="T72" s="32"/>
       <c r="U72" s="28"/>
       <c r="V72" s="28"/>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>346</v>
       </c>
@@ -5377,78 +5720,78 @@
       <c r="N73" s="13"/>
       <c r="O73" s="13"/>
       <c r="P73" s="13"/>
-      <c r="Q73" s="34"/>
-      <c r="R73" s="34"/>
-      <c r="S73" s="34"/>
+      <c r="Q73" s="33"/>
+      <c r="R73" s="33"/>
+      <c r="S73" s="33"/>
       <c r="T73" s="13"/>
       <c r="U73" s="13"/>
       <c r="V73" s="13"/>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B74" s="38" t="s">
+      <c r="B74" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C74" s="40"/>
-      <c r="D74" s="41"/>
-      <c r="E74" s="38" t="s">
+      <c r="C74" s="63"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="F74" s="40"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="38" t="s">
+      <c r="F74" s="63"/>
+      <c r="G74" s="64"/>
+      <c r="H74" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="I74" s="40"/>
-      <c r="J74" s="41"/>
-      <c r="K74" s="38" t="s">
+      <c r="I74" s="63"/>
+      <c r="J74" s="64"/>
+      <c r="K74" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="L74" s="40"/>
-      <c r="M74" s="41"/>
-      <c r="N74" s="38" t="s">
+      <c r="L74" s="63"/>
+      <c r="M74" s="64"/>
+      <c r="N74" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="O74" s="40"/>
-      <c r="P74" s="41"/>
-      <c r="Q74" s="38" t="s">
+      <c r="O74" s="63"/>
+      <c r="P74" s="64"/>
+      <c r="Q74" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="R74" s="40"/>
-      <c r="S74" s="41"/>
-      <c r="T74" s="38" t="s">
+      <c r="R74" s="63"/>
+      <c r="S74" s="64"/>
+      <c r="T74" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="U74" s="40"/>
-      <c r="V74" s="41"/>
-    </row>
-    <row r="75" spans="1:22">
+      <c r="U74" s="63"/>
+      <c r="V74" s="64"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="16"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="42"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="42"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="42"/>
-      <c r="J75" s="43"/>
-      <c r="K75" s="39"/>
-      <c r="L75" s="42"/>
-      <c r="M75" s="43"/>
-      <c r="N75" s="39"/>
-      <c r="O75" s="42"/>
-      <c r="P75" s="43"/>
-      <c r="Q75" s="39"/>
-      <c r="R75" s="42"/>
-      <c r="S75" s="43"/>
-      <c r="T75" s="39"/>
-      <c r="U75" s="42"/>
-      <c r="V75" s="43"/>
-    </row>
-    <row r="76" spans="1:22">
+      <c r="B75" s="62"/>
+      <c r="C75" s="65"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="62"/>
+      <c r="F75" s="65"/>
+      <c r="G75" s="66"/>
+      <c r="H75" s="62"/>
+      <c r="I75" s="65"/>
+      <c r="J75" s="66"/>
+      <c r="K75" s="62"/>
+      <c r="L75" s="65"/>
+      <c r="M75" s="66"/>
+      <c r="N75" s="62"/>
+      <c r="O75" s="65"/>
+      <c r="P75" s="66"/>
+      <c r="Q75" s="62"/>
+      <c r="R75" s="65"/>
+      <c r="S75" s="66"/>
+      <c r="T75" s="62"/>
+      <c r="U75" s="65"/>
+      <c r="V75" s="66"/>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>38</v>
       </c>
@@ -5516,7 +5859,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="77" spans="1:22">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
@@ -5540,7 +5883,7 @@
       <c r="U77" s="19"/>
       <c r="V77" s="19"/>
     </row>
-    <row r="78" spans="1:22">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
@@ -5564,7 +5907,7 @@
       <c r="U78" s="19"/>
       <c r="V78" s="19"/>
     </row>
-    <row r="79" spans="1:22" ht="15.95" customHeight="1">
+    <row r="79" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
@@ -5588,7 +5931,7 @@
       <c r="U79" s="19"/>
       <c r="V79" s="19"/>
     </row>
-    <row r="80" spans="1:22">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80" s="20"/>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
@@ -5612,7 +5955,7 @@
       <c r="U80" s="19"/>
       <c r="V80" s="19"/>
     </row>
-    <row r="81" spans="1:22">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A81" s="20"/>
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
@@ -5636,7 +5979,7 @@
       <c r="U81" s="19"/>
       <c r="V81" s="19"/>
     </row>
-    <row r="82" spans="1:22">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82" s="20"/>
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
@@ -5660,7 +6003,7 @@
       <c r="U82" s="19"/>
       <c r="V82" s="19"/>
     </row>
-    <row r="83" spans="1:22">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83" s="20"/>
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
@@ -5684,7 +6027,7 @@
       <c r="U83" s="19"/>
       <c r="V83" s="19"/>
     </row>
-    <row r="84" spans="1:22">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A84" s="20"/>
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
@@ -5708,7 +6051,7 @@
       <c r="U84" s="19"/>
       <c r="V84" s="19"/>
     </row>
-    <row r="85" spans="1:22">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A85" s="20"/>
       <c r="B85" s="19"/>
       <c r="C85" s="19"/>
@@ -5732,7 +6075,7 @@
       <c r="U85" s="19"/>
       <c r="V85" s="19"/>
     </row>
-    <row r="86" spans="1:22">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" s="20"/>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -5756,7 +6099,7 @@
       <c r="U86" s="19"/>
       <c r="V86" s="19"/>
     </row>
-    <row r="87" spans="1:22">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87" s="20"/>
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
@@ -5780,7 +6123,7 @@
       <c r="U87" s="19"/>
       <c r="V87" s="19"/>
     </row>
-    <row r="88" spans="1:22">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88" s="20"/>
       <c r="B88" s="19"/>
       <c r="C88" s="19"/>
@@ -5804,7 +6147,7 @@
       <c r="U88" s="19"/>
       <c r="V88" s="19"/>
     </row>
-    <row r="89" spans="1:22">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89" s="20"/>
       <c r="B89" s="19"/>
       <c r="C89" s="19"/>
@@ -5828,7 +6171,7 @@
       <c r="U89" s="19"/>
       <c r="V89" s="19"/>
     </row>
-    <row r="90" spans="1:22">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90" s="20"/>
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
@@ -5852,7 +6195,7 @@
       <c r="U90" s="19"/>
       <c r="V90" s="19"/>
     </row>
-    <row r="91" spans="1:22">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
       <c r="B91" s="19"/>
       <c r="C91" s="19"/>
@@ -5876,7 +6219,7 @@
       <c r="U91" s="19"/>
       <c r="V91" s="19"/>
     </row>
-    <row r="92" spans="1:22">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92" s="20"/>
       <c r="B92" s="19"/>
       <c r="C92" s="19"/>
@@ -5900,7 +6243,7 @@
       <c r="U92" s="19"/>
       <c r="V92" s="19"/>
     </row>
-    <row r="93" spans="1:22">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93" s="20"/>
       <c r="B93" s="19"/>
       <c r="C93" s="19"/>
@@ -5924,7 +6267,7 @@
       <c r="U93" s="19"/>
       <c r="V93" s="19"/>
     </row>
-    <row r="94" spans="1:22">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94" s="20"/>
       <c r="B94" s="19"/>
       <c r="C94" s="19"/>
@@ -5948,7 +6291,7 @@
       <c r="U94" s="19"/>
       <c r="V94" s="19"/>
     </row>
-    <row r="95" spans="1:22">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A95" s="20"/>
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
@@ -5972,7 +6315,7 @@
       <c r="U95" s="19"/>
       <c r="V95" s="19"/>
     </row>
-    <row r="96" spans="1:22">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A96" s="20"/>
       <c r="B96" s="19"/>
       <c r="C96" s="19"/>
@@ -5996,7 +6339,7 @@
       <c r="U96" s="19"/>
       <c r="V96" s="19"/>
     </row>
-    <row r="97" spans="1:22">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A97" s="20"/>
       <c r="B97" s="19"/>
       <c r="C97" s="19"/>
@@ -6020,7 +6363,7 @@
       <c r="U97" s="19"/>
       <c r="V97" s="19"/>
     </row>
-    <row r="98" spans="1:22">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98" s="20"/>
       <c r="B98" s="19"/>
       <c r="C98" s="19"/>
@@ -6044,7 +6387,7 @@
       <c r="U98" s="19"/>
       <c r="V98" s="19"/>
     </row>
-    <row r="99" spans="1:22">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A99" s="20"/>
       <c r="B99" s="19"/>
       <c r="C99" s="19"/>
@@ -6068,7 +6411,7 @@
       <c r="U99" s="19"/>
       <c r="V99" s="19"/>
     </row>
-    <row r="100" spans="1:22">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A100" s="20"/>
       <c r="B100" s="19"/>
       <c r="C100" s="19"/>
@@ -6092,7 +6435,7 @@
       <c r="U100" s="19"/>
       <c r="V100" s="19"/>
     </row>
-    <row r="101" spans="1:22">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A101" s="20"/>
       <c r="B101" s="19"/>
       <c r="C101" s="19"/>
@@ -6116,7 +6459,7 @@
       <c r="U101" s="19"/>
       <c r="V101" s="19"/>
     </row>
-    <row r="102" spans="1:22">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A102" s="20"/>
       <c r="B102" s="19"/>
       <c r="C102" s="19"/>
@@ -6140,7 +6483,7 @@
       <c r="U102" s="19"/>
       <c r="V102" s="19"/>
     </row>
-    <row r="103" spans="1:22">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A103" s="20"/>
       <c r="B103" s="19"/>
       <c r="C103" s="19"/>
@@ -6164,7 +6507,7 @@
       <c r="U103" s="19"/>
       <c r="V103" s="19"/>
     </row>
-    <row r="104" spans="1:22">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A104" s="20"/>
       <c r="B104" s="19"/>
       <c r="C104" s="19"/>
@@ -6188,7 +6531,7 @@
       <c r="U104" s="19"/>
       <c r="V104" s="19"/>
     </row>
-    <row r="105" spans="1:22">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A105" s="20"/>
       <c r="B105" s="19"/>
       <c r="C105" s="19"/>
@@ -6212,7 +6555,7 @@
       <c r="U105" s="19"/>
       <c r="V105" s="19"/>
     </row>
-    <row r="106" spans="1:22">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A106" s="20"/>
       <c r="B106" s="19"/>
       <c r="C106" s="19"/>
@@ -6236,7 +6579,7 @@
       <c r="U106" s="19"/>
       <c r="V106" s="19"/>
     </row>
-    <row r="107" spans="1:22">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A107" s="20"/>
       <c r="B107" s="19"/>
       <c r="C107" s="19"/>
@@ -6260,7 +6603,7 @@
       <c r="U107" s="19"/>
       <c r="V107" s="19"/>
     </row>
-    <row r="108" spans="1:22">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A108" s="20"/>
       <c r="B108" s="19"/>
       <c r="C108" s="19"/>
@@ -6284,7 +6627,7 @@
       <c r="U108" s="19"/>
       <c r="V108" s="19"/>
     </row>
-    <row r="109" spans="1:22">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A109" s="20"/>
       <c r="B109" s="19"/>
       <c r="C109" s="19"/>
@@ -6308,7 +6651,7 @@
       <c r="U109" s="19"/>
       <c r="V109" s="19"/>
     </row>
-    <row r="110" spans="1:22">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A110" s="20"/>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
@@ -6332,7 +6675,7 @@
       <c r="U110" s="19"/>
       <c r="V110" s="19"/>
     </row>
-    <row r="111" spans="1:22">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A111" s="20"/>
       <c r="B111" s="19"/>
       <c r="C111" s="19"/>
@@ -6356,7 +6699,7 @@
       <c r="U111" s="19"/>
       <c r="V111" s="19"/>
     </row>
-    <row r="112" spans="1:22">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A112" s="20"/>
       <c r="B112" s="19"/>
       <c r="C112" s="19"/>
@@ -6380,7 +6723,7 @@
       <c r="U112" s="19"/>
       <c r="V112" s="19"/>
     </row>
-    <row r="113" spans="1:22">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A113" s="20"/>
       <c r="B113" s="19"/>
       <c r="C113" s="19"/>
@@ -6404,7 +6747,7 @@
       <c r="U113" s="19"/>
       <c r="V113" s="19"/>
     </row>
-    <row r="114" spans="1:22">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A114" s="20"/>
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
@@ -6428,7 +6771,7 @@
       <c r="U114" s="19"/>
       <c r="V114" s="19"/>
     </row>
-    <row r="115" spans="1:22">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A115" s="20"/>
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
@@ -6452,7 +6795,7 @@
       <c r="U115" s="19"/>
       <c r="V115" s="19"/>
     </row>
-    <row r="116" spans="1:22">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A116" s="20"/>
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
@@ -6478,6 +6821,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="T74:T75"/>
+    <mergeCell ref="U74:V75"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="O74:P75"/>
+    <mergeCell ref="Q74:Q75"/>
+    <mergeCell ref="R74:S75"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:G75"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="I74:J75"/>
+    <mergeCell ref="K74:K75"/>
+    <mergeCell ref="L74:M75"/>
+    <mergeCell ref="N74:N75"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="L15:M15"/>
     <mergeCell ref="U14:V14"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
@@ -6494,29 +6860,6 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="L14:M14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:G75"/>
-    <mergeCell ref="H74:H75"/>
-    <mergeCell ref="I74:J75"/>
-    <mergeCell ref="K74:K75"/>
-    <mergeCell ref="L74:M75"/>
-    <mergeCell ref="N74:N75"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="T74:T75"/>
-    <mergeCell ref="U74:V75"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="O74:P75"/>
-    <mergeCell ref="Q74:Q75"/>
-    <mergeCell ref="R74:S75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6688,6 +7031,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="4b4900cf-16f2-4e92-b6c2-051ea2da4c63">
@@ -6701,23 +7053,39 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F6E84E-A27F-4043-9FC3-A9C50EEB8300}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F6E84E-A27F-4043-9FC3-A9C50EEB8300}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="921ea608-9a9c-45f0-ad48-b556cc379e8f"/>
+    <ds:schemaRef ds:uri="4b4900cf-16f2-4e92-b6c2-051ea2da4c63"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1CEBFF-FDE4-4175-8251-FD0DF8B45305}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9452A3-D376-4675-95FF-4BF41E3CA5BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9452A3-D376-4675-95FF-4BF41E3CA5BB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1CEBFF-FDE4-4175-8251-FD0DF8B45305}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4b4900cf-16f2-4e92-b6c2-051ea2da4c63"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating broadcast_listeners flows and apis
</commit_message>
<xml_diff>
--- a/docs/flow/broadcast_partner_information.xlsx
+++ b/docs/flow/broadcast_partner_information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunoric/Devel/Smartbox/millenniumfalcon/r2-d2-api/docs/flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65236F59-E82C-4A4C-BBDB-85B04FAE09CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF2CC6B-AC0E-CA4E-B628-984A483E40A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4800" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="353">
   <si>
     <t>Integration Information</t>
   </si>
@@ -1086,10 +1086,13 @@
     <t>/broadcast_listerners/partners</t>
   </si>
   <si>
-    <t>smartbox_id</t>
-  </si>
-  <si>
     <t>partners</t>
+  </si>
+  <si>
+    <t>golden_id</t>
+  </si>
+  <si>
+    <t>cease_date</t>
   </si>
 </sst>
 </file>
@@ -1725,6 +1728,30 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1818,30 +1845,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -2131,8 +2134,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q19" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U71" sqref="U71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2147,41 +2151,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2190,34 +2194,34 @@
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="56"/>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2240,14 +2244,14 @@
       <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="56"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -2267,14 +2271,14 @@
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="59"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="65"/>
       <c r="H8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2283,27 +2287,27 @@
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="50"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="2" t="s">
         <v>18</v>
       </c>
@@ -2312,14 +2316,14 @@
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="2" t="s">
         <v>21</v>
       </c>
@@ -2359,52 +2363,52 @@
       <c r="B14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="37" t="s">
+      <c r="I14" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="38"/>
+      <c r="J14" s="44"/>
       <c r="K14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="37" t="s">
+      <c r="L14" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="38"/>
+      <c r="M14" s="44"/>
       <c r="N14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="37" t="s">
+      <c r="O14" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="P14" s="38"/>
+      <c r="P14" s="44"/>
       <c r="Q14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="R14" s="37" t="s">
+      <c r="R14" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="S14" s="38"/>
+      <c r="S14" s="44"/>
       <c r="T14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="U14" s="37" t="s">
+      <c r="U14" s="43" t="s">
         <v>348</v>
       </c>
-      <c r="V14" s="38"/>
+      <c r="V14" s="44"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
@@ -2413,48 +2417,48 @@
       <c r="B15" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="44"/>
       <c r="H15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="44"/>
       <c r="K15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="38"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="44"/>
       <c r="N15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="O15" s="37" t="s">
+      <c r="O15" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="P15" s="38"/>
+      <c r="P15" s="44"/>
       <c r="Q15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="R15" s="37" t="s">
+      <c r="R15" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="S15" s="38"/>
+      <c r="S15" s="44"/>
       <c r="T15" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="U15" s="37" t="s">
+      <c r="U15" s="43" t="s">
         <v>349</v>
       </c>
-      <c r="V15" s="38"/>
+      <c r="V15" s="44"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -2575,13 +2579,13 @@
       </c>
       <c r="S17" s="20"/>
       <c r="T17" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="U17" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="U17" s="19" t="s">
-        <v>350</v>
-      </c>
       <c r="V17" s="19" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -2753,7 +2757,7 @@
       </c>
       <c r="S20" s="20"/>
       <c r="T20" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U20" s="19" t="s">
         <v>64</v>
@@ -2989,7 +2993,7 @@
       </c>
       <c r="S24" s="20"/>
       <c r="T24" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="U24" s="19" t="s">
         <v>90</v>
@@ -5616,13 +5620,13 @@
       </c>
       <c r="S70" s="34"/>
       <c r="T70" s="19" t="s">
-        <v>62</v>
+        <v>350</v>
       </c>
       <c r="U70" s="19" t="s">
-        <v>62</v>
+        <v>352</v>
       </c>
       <c r="V70" s="19" t="s">
-        <v>62</v>
+        <v>352</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
@@ -5731,65 +5735,65 @@
       <c r="A74" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B74" s="61" t="s">
+      <c r="B74" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C74" s="63"/>
-      <c r="D74" s="64"/>
-      <c r="E74" s="61" t="s">
+      <c r="C74" s="39"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="F74" s="63"/>
-      <c r="G74" s="64"/>
-      <c r="H74" s="61" t="s">
+      <c r="F74" s="39"/>
+      <c r="G74" s="40"/>
+      <c r="H74" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I74" s="63"/>
-      <c r="J74" s="64"/>
-      <c r="K74" s="61" t="s">
+      <c r="I74" s="39"/>
+      <c r="J74" s="40"/>
+      <c r="K74" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="L74" s="63"/>
-      <c r="M74" s="64"/>
-      <c r="N74" s="61" t="s">
+      <c r="L74" s="39"/>
+      <c r="M74" s="40"/>
+      <c r="N74" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="O74" s="63"/>
-      <c r="P74" s="64"/>
-      <c r="Q74" s="61" t="s">
+      <c r="O74" s="39"/>
+      <c r="P74" s="40"/>
+      <c r="Q74" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="R74" s="63"/>
-      <c r="S74" s="64"/>
-      <c r="T74" s="61" t="s">
+      <c r="R74" s="39"/>
+      <c r="S74" s="40"/>
+      <c r="T74" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="U74" s="63"/>
-      <c r="V74" s="64"/>
+      <c r="U74" s="39"/>
+      <c r="V74" s="40"/>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="16"/>
-      <c r="B75" s="62"/>
-      <c r="C75" s="65"/>
-      <c r="D75" s="66"/>
-      <c r="E75" s="62"/>
-      <c r="F75" s="65"/>
-      <c r="G75" s="66"/>
-      <c r="H75" s="62"/>
-      <c r="I75" s="65"/>
-      <c r="J75" s="66"/>
-      <c r="K75" s="62"/>
-      <c r="L75" s="65"/>
-      <c r="M75" s="66"/>
-      <c r="N75" s="62"/>
-      <c r="O75" s="65"/>
-      <c r="P75" s="66"/>
-      <c r="Q75" s="62"/>
-      <c r="R75" s="65"/>
-      <c r="S75" s="66"/>
-      <c r="T75" s="62"/>
-      <c r="U75" s="65"/>
-      <c r="V75" s="66"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="41"/>
+      <c r="G75" s="42"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="41"/>
+      <c r="J75" s="42"/>
+      <c r="K75" s="38"/>
+      <c r="L75" s="41"/>
+      <c r="M75" s="42"/>
+      <c r="N75" s="38"/>
+      <c r="O75" s="41"/>
+      <c r="P75" s="42"/>
+      <c r="Q75" s="38"/>
+      <c r="R75" s="41"/>
+      <c r="S75" s="42"/>
+      <c r="T75" s="38"/>
+      <c r="U75" s="41"/>
+      <c r="V75" s="42"/>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -6821,13 +6825,22 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="T74:T75"/>
-    <mergeCell ref="U74:V75"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="O74:P75"/>
-    <mergeCell ref="Q74:Q75"/>
-    <mergeCell ref="R74:S75"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="L14:M14"/>
     <mergeCell ref="O14:P14"/>
     <mergeCell ref="R14:S14"/>
     <mergeCell ref="U15:V15"/>
@@ -6844,28 +6857,42 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="L15:M15"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="T74:T75"/>
+    <mergeCell ref="U74:V75"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="O74:P75"/>
+    <mergeCell ref="Q74:Q75"/>
+    <mergeCell ref="R74:S75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="4b4900cf-16f2-4e92-b6c2-051ea2da4c63">
+      <UserInfo>
+        <DisplayName>Aleksandra Sadowska</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EB1F655CC7BD0742810412331548437C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="47ba522df40ebb04e30b9f2a6350b81c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="921ea608-9a9c-45f0-ad48-b556cc379e8f" xmlns:ns3="4b4900cf-16f2-4e92-b6c2-051ea2da4c63" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="28604ed46e357d4f4143d69e0a75604c" ns2:_="" ns3:_="">
     <xsd:import namespace="921ea608-9a9c-45f0-ad48-b556cc379e8f"/>
@@ -7030,30 +7057,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1CEBFF-FDE4-4175-8251-FD0DF8B45305}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4b4900cf-16f2-4e92-b6c2-051ea2da4c63"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="4b4900cf-16f2-4e92-b6c2-051ea2da4c63">
-      <UserInfo>
-        <DisplayName>Aleksandra Sadowska</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9452A3-D376-4675-95FF-4BF41E3CA5BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F6E84E-A27F-4043-9FC3-A9C50EEB8300}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7070,22 +7092,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9452A3-D376-4675-95FF-4BF41E3CA5BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1CEBFF-FDE4-4175-8251-FD0DF8B45305}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4b4900cf-16f2-4e92-b6c2-051ea2da4c63"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>